<commit_message>
Primeira etapa do projeto
</commit_message>
<xml_diff>
--- a/nomes/NOMES.xlsx
+++ b/nomes/NOMES.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thalissa.mariana\Documents\PROJETOS THALISSA\PROJETOS\projeto_email\nomes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880B5A12-582A-46D7-A846-103BD71929E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F093A2-C553-46E7-B57A-AB7488A90D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FBBBD53-5718-4F7B-A1F8-84F9A2CB3253}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2FBBBD53-5718-4F7B-A1F8-84F9A2CB3253}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="contatos" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">contatos!$A$2:$D$15</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,11 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
-  <si>
-    <t xml:space="preserve">AUTOSSERVIÇO </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="130">
   <si>
     <t xml:space="preserve">COORD ABEL </t>
   </si>
@@ -312,13 +335,130 @@
   </si>
   <si>
     <t>COORD ADILSON ESPOSITO</t>
+  </si>
+  <si>
+    <t>Nomes</t>
+  </si>
+  <si>
+    <t>REGIOES</t>
+  </si>
+  <si>
+    <t>VAREJO - NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STARMAX </t>
+  </si>
+  <si>
+    <t>VAREJO</t>
+  </si>
+  <si>
+    <t>STAR MAX - NE</t>
+  </si>
+  <si>
+    <t>VAREJO - MG</t>
+  </si>
+  <si>
+    <t>STAR MAX - MG</t>
+  </si>
+  <si>
+    <t>VAREJO - RJ</t>
+  </si>
+  <si>
+    <t>STAR MAX - RJ</t>
+  </si>
+  <si>
+    <t>VAREJO - SPI</t>
+  </si>
+  <si>
+    <t>STAR MAX - SPI</t>
+  </si>
+  <si>
+    <t>VAREJO - SUL</t>
+  </si>
+  <si>
+    <t>STAR MAX - SUL</t>
+  </si>
+  <si>
+    <t>VAREJO - SPC</t>
+  </si>
+  <si>
+    <t>STAR MAX - SPC</t>
+  </si>
+  <si>
+    <t>VAREJO - BA</t>
+  </si>
+  <si>
+    <t>STAR MAX - BA</t>
+  </si>
+  <si>
+    <t>KA REGIONAL</t>
+  </si>
+  <si>
+    <t>TELEVENDAS</t>
+  </si>
+  <si>
+    <t>AUTOSSERVIÇO</t>
+  </si>
+  <si>
+    <t>VAREJO - CO</t>
+  </si>
+  <si>
+    <t>STAR MAX - CO</t>
+  </si>
+  <si>
+    <t>VAREJO - IND. NO</t>
+  </si>
+  <si>
+    <t>STAR MAX - IND. NO</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>andreza.ferreira@adimax.com.br</t>
+  </si>
+  <si>
+    <t>alexandre.barbosa@adimax.com.br</t>
+  </si>
+  <si>
+    <t>Fernando.Braga@adimax.com.br</t>
+  </si>
+  <si>
+    <t>ricardo.maas@adimax.com.br</t>
+  </si>
+  <si>
+    <t>wilian.bataglioli@adimax.com.br</t>
+  </si>
+  <si>
+    <t>allan.guarnieri@adimax.com.br</t>
+  </si>
+  <si>
+    <t>renato.aguiar@adimax.com.br</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vago </t>
+  </si>
+  <si>
+    <t>alex.freitas@adimax.com.br</t>
+  </si>
+  <si>
+    <t>agenor.moreira@adimax.com.br</t>
+  </si>
+  <si>
+    <t>camila.galastri@adimax.com.br</t>
+  </si>
+  <si>
+    <t>erick.bez@adimax.com.br</t>
+  </si>
+  <si>
+    <t>camila.campos@adimax.com.br</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,16 +466,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -343,14 +511,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -683,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4325C4-1102-403A-AE31-3D2F68A1E175}">
-  <dimension ref="A1:A92"/>
+  <dimension ref="A2:A92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,467 +903,728 @@
     <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368BD947-634D-4CD1-AACF-98B86BB9E0B9}">
+  <dimension ref="A2:E15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A3" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C2,$A$2:$A$272),0))</f>
+        <v>ANDREZA FERREIRA</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A4" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C3,$A$2:$A$272),0))</f>
+        <v>ALEXANDRE BARBOSA</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A5" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C4,$A$2:$A$272),0))</f>
+        <v>FERNANDO BRAGA</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A6" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C5,$A$2:$A$272),0))</f>
+        <v>RICARDO MAAS</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A7" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C6,$A$2:$A$272),0))</f>
+        <v>WILIAN BATAGLIOLI</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A8" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C7,$A$2:$A$272),0))</f>
+        <v>ALLAN GUARNIERI</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A9" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C8,$A$2:$A$272),0))</f>
+        <v>RENATO AGUIAR</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A10" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C9,$A$2:$A$272),0))</f>
+        <v>GUSTAVO HENRIQUE</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A11" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C10,$A$2:$A$272),0))</f>
+        <v>ALEX FREITAS</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A12" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C11,$A$2:$A$272),0))</f>
+        <v>AGENOR MOREIRA</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A13" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C12,$A$2:$A$272),0))</f>
+        <v>CAMILA GALASTRI</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A14" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C13,$A$2:$A$272),0))</f>
+        <v>ERICK BEZ</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="str" cm="1">
+        <f t="array" aca="1" ref="A15" ca="1">INDEX($A$2:$A$272,MATCH(0,COUNTIF(A$1:$C14,$A$2:$A$272),0))</f>
+        <v>CAMILA CAMPOS</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:D15" xr:uid="{368BD947-634D-4CD1-AACF-98B86BB9E0B9}"/>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{7808D911-64A0-45E5-BCC6-74890147E8D0}"/>
+    <hyperlink ref="E6" r:id="rId2" display="andreza.ferreira@adimax.com.br" xr:uid="{E550B96C-2521-4E69-849B-3026E664B009}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{656A31CD-B140-4928-9A89-03D559FCE46C}"/>
+    <hyperlink ref="E9" r:id="rId4" display="andreza.ferreira@adimax.com.br" xr:uid="{BAE5E790-F9B1-4386-AA53-B116A6301B0A}"/>
+    <hyperlink ref="E11" r:id="rId5" display="alexandre.barbosa@adimax.com.br" xr:uid="{1D0EA750-E60C-4388-8083-22431E55F7F8}"/>
+    <hyperlink ref="E12" r:id="rId6" display="renato.aguiar@adimax.com.br" xr:uid="{7E529294-F3A7-47E9-8969-2667FB125F3A}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{0CBD3632-9839-4A39-9DC0-004085B0CDC3}"/>
+    <hyperlink ref="E14" r:id="rId8" display="allan.guarnieri@adimax.com.br" xr:uid="{874D3A16-2146-4822-B114-9CF7934B7534}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>